<commit_message>
Incluida variable Area_bolanha en las listas
</commit_message>
<xml_diff>
--- a/Pruebas/resultados_observados_vs_predichos.xlsx
+++ b/Pruebas/resultados_observados_vs_predichos.xlsx
@@ -1,13 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>

</xml_diff>

<commit_message>
+ Area_bolanha in rf
</commit_message>
<xml_diff>
--- a/Pruebas/resultados_observados_vs_predichos.xlsx
+++ b/Pruebas/resultados_observados_vs_predichos.xlsx
@@ -466,7 +466,7 @@
         <v>19</v>
       </c>
       <c r="B4" t="n">
-        <v>16</v>
+        <v>17</v>
       </c>
     </row>
     <row r="5">
@@ -490,7 +490,7 @@
         <v>12</v>
       </c>
       <c r="B7" t="n">
-        <v>10</v>
+        <v>8</v>
       </c>
     </row>
     <row r="8">
@@ -498,7 +498,7 @@
         <v>19</v>
       </c>
       <c r="B8" t="n">
-        <v>17</v>
+        <v>18</v>
       </c>
     </row>
     <row r="9">
@@ -506,7 +506,7 @@
         <v>7</v>
       </c>
       <c r="B9" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="10">
@@ -514,7 +514,7 @@
         <v>19</v>
       </c>
       <c r="B10" t="n">
-        <v>17</v>
+        <v>15</v>
       </c>
     </row>
     <row r="11">
@@ -546,7 +546,7 @@
         <v>4</v>
       </c>
       <c r="B14" t="n">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="15">
@@ -554,7 +554,7 @@
         <v>19</v>
       </c>
       <c r="B15" t="n">
-        <v>10</v>
+        <v>8</v>
       </c>
     </row>
     <row r="16">
@@ -562,7 +562,7 @@
         <v>4</v>
       </c>
       <c r="B16" t="n">
-        <v>5</v>
+        <v>7</v>
       </c>
     </row>
     <row r="17">
@@ -570,7 +570,7 @@
         <v>9</v>
       </c>
       <c r="B17" t="n">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="18">
@@ -586,7 +586,7 @@
         <v>19</v>
       </c>
       <c r="B19" t="n">
-        <v>18</v>
+        <v>16</v>
       </c>
     </row>
     <row r="20">
@@ -618,7 +618,7 @@
         <v>9</v>
       </c>
       <c r="B23" t="n">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="24">
@@ -634,7 +634,7 @@
         <v>19</v>
       </c>
       <c r="B25" t="n">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="26">
@@ -642,7 +642,7 @@
         <v>9</v>
       </c>
       <c r="B26" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="27">

</xml_diff>